<commit_message>
My single function version
</commit_message>
<xml_diff>
--- a/CH-046 Numbers Cleaning.xlsx
+++ b/CH-046 Numbers Cleaning.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://starkeyhearingtechnologies-my.sharepoint.com/personal/mark_biegert_starkey_com/Documents/Desktop/Toss/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FD4EBCA-6290-439D-ABD0-FE18E552ED58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2486585E-5790-489E-9E85-3734EE3CC9E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="1665" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$2:$B$16</definedName>
+    <definedName name="_nR">Sheet1!$T$9:$T$22</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -343,14 +344,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="3" fontId="2" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="3" fontId="2" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="3" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="3" fontId="2" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="3" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -813,6 +814,50 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>194797</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>110656</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4F9B1605-BF9A-63CF-D3C1-C5BEAD63CDE0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7562850" y="4600575"/>
+          <a:ext cx="5624047" cy="1920406"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1133,10 +1178,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:Y75"/>
+  <dimension ref="B1:AA75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20:J22"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1144,6 +1189,7 @@
     <col min="1" max="1" width="3.33203125" customWidth="1"/>
     <col min="2" max="2" width="15" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5.109375" customWidth="1"/>
+    <col min="9" max="9" width="11.109375" customWidth="1"/>
     <col min="10" max="10" width="10.44140625" bestFit="1" customWidth="1"/>
     <col min="11" max="14" width="10.44140625" customWidth="1"/>
     <col min="16" max="16" width="11.33203125" customWidth="1"/>
@@ -1151,7 +1197,7 @@
     <col min="23" max="23" width="8.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:25" s="4" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:27" s="4" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1163,7 +1209,7 @@
       <c r="M1" s="20"/>
       <c r="N1" s="20"/>
     </row>
-    <row r="2" spans="2:25" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:27" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B2" s="8" t="s">
         <v>5</v>
       </c>
@@ -1175,7 +1221,7 @@
       <c r="M2" s="21"/>
       <c r="N2" s="21"/>
     </row>
-    <row r="3" spans="2:25" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:27" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B3" s="13">
         <v>1006</v>
       </c>
@@ -1187,7 +1233,7 @@
       <c r="M3" s="22"/>
       <c r="N3" s="22"/>
     </row>
-    <row r="4" spans="2:25" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:27" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B4" s="11">
         <v>1003</v>
       </c>
@@ -1199,7 +1245,7 @@
       <c r="M4" s="23"/>
       <c r="N4" s="23"/>
     </row>
-    <row r="5" spans="2:25" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:27" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B5" s="9">
         <v>1016</v>
       </c>
@@ -1212,7 +1258,7 @@
       <c r="M5" s="24"/>
       <c r="N5" s="24"/>
     </row>
-    <row r="6" spans="2:25" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:27" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B6" s="12">
         <v>1013</v>
       </c>
@@ -1226,7 +1272,7 @@
       <c r="N6" s="25"/>
       <c r="P6" s="5"/>
     </row>
-    <row r="7" spans="2:25" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:27" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B7" s="9">
         <v>1018</v>
       </c>
@@ -1235,895 +1281,1006 @@
       <c r="J7" s="19">
         <v>1018</v>
       </c>
-      <c r="K7" s="26"/>
-      <c r="L7" s="26"/>
+      <c r="K7" s="31"/>
+      <c r="L7" s="31"/>
       <c r="M7" s="25"/>
-      <c r="N7" s="25" t="s">
+      <c r="N7" s="25"/>
+      <c r="O7" s="25"/>
+      <c r="P7" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="O7" s="2" t="s">
+      <c r="Q7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="P7" s="2" t="s">
+      <c r="R7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="Q7" s="2" t="s">
+      <c r="S7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="R7" s="5"/>
-    </row>
-    <row r="8" spans="2:25" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="T7" s="5"/>
+    </row>
+    <row r="8" spans="2:27" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B8" s="12">
         <v>1008</v>
       </c>
       <c r="D8"/>
-      <c r="O8" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="P8" s="2" t="b">
-        <v>0</v>
+      <c r="K8" s="2">
+        <v>999</v>
       </c>
       <c r="Q8" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="R8" s="5">
+      <c r="R8" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="S8" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="T8" s="5">
         <v>1000</v>
       </c>
     </row>
-    <row r="9" spans="2:25" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:27" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B9" s="11">
         <v>1001</v>
       </c>
       <c r="D9"/>
-      <c r="J9"/>
-      <c r="K9" s="28">
-        <f t="shared" ref="K9:K22" si="0">R9-R8</f>
-        <v>1</v>
-      </c>
-      <c r="L9" s="2">
-        <f>R10-R9</f>
-        <v>1</v>
-      </c>
-      <c r="M9" s="5">
-        <f>N9+M8</f>
-        <v>0</v>
-      </c>
-      <c r="N9" s="5">
-        <f>--OR(O9,NOT(OR(O9:Q9)))</f>
-        <v>0</v>
-      </c>
-      <c r="O9" s="5" t="b">
-        <f>AND(R10-R9=1,NOT(P9))</f>
-        <v>0</v>
-      </c>
-      <c r="P9" s="2" t="b">
-        <f>AND((R10-R9)=1,R9-R8=1)</f>
-        <v>1</v>
-      </c>
-      <c r="Q9" s="2" t="b">
-        <f>AND((R10-R9&lt;&gt;1),OR(O8,P8))</f>
-        <v>0</v>
-      </c>
-      <c r="R9" s="2" cm="1">
-        <f t="array" ref="R9:R22">_xlfn._xlws.SORT(B3:B16)</f>
+      <c r="J9">
+        <f>SUM(K9+J8)</f>
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <f>IF(T9-T8&gt;1,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="L9"/>
+      <c r="M9" s="27">
+        <f t="shared" ref="M9:M22" si="0">T9-T8</f>
+        <v>1</v>
+      </c>
+      <c r="N9" s="2">
+        <f>T10-T9</f>
+        <v>1</v>
+      </c>
+      <c r="O9" s="5">
+        <f>P9+O8</f>
+        <v>0</v>
+      </c>
+      <c r="P9" s="5">
+        <f>--OR(Q9,NOT(OR(Q9:S9)))</f>
+        <v>0</v>
+      </c>
+      <c r="Q9" s="5" t="b">
+        <f>AND(T10-T9=1,NOT(R9))</f>
+        <v>0</v>
+      </c>
+      <c r="R9" s="2" t="b">
+        <f>AND((T10-T9)=1,T9-T8=1)</f>
+        <v>1</v>
+      </c>
+      <c r="S9" s="2" t="b">
+        <f>AND((T10-T9&lt;&gt;1),OR(Q8,R8))</f>
+        <v>0</v>
+      </c>
+      <c r="T9" s="2" cm="1">
+        <f t="array" ref="T9:T22">_xlfn._xlws.SORT(B3:B16)</f>
         <v>1001</v>
       </c>
-      <c r="S9" s="5">
-        <f>M9</f>
-        <v>0</v>
-      </c>
-      <c r="T9" s="2" cm="1">
-        <f t="array" ref="T9:T13">_xlfn.UNIQUE(S9:S22)</f>
-        <v>0</v>
-      </c>
-      <c r="U9" s="2">
-        <f>_xlfn.XMATCH(T9,$S$9:$S$22,,-1)</f>
+      <c r="U9" s="5">
+        <f>O9</f>
+        <v>0</v>
+      </c>
+      <c r="V9" s="2" cm="1">
+        <f t="array" ref="V9:V13">_xlfn.UNIQUE(U9:U22)</f>
+        <v>0</v>
+      </c>
+      <c r="W9" s="2">
+        <f>_xlfn.XMATCH(V9,$U$9:$U$22,,-1)</f>
         <v>4</v>
       </c>
-      <c r="V9" s="2">
-        <f>_xlfn.XMATCH(T9,$S$9:$S$22,,1)</f>
-        <v>1</v>
-      </c>
-      <c r="W9" s="2" cm="1">
-        <f t="array" ref="W9">INDEX(_xlfn.ANCHORARRAY($R$9),U9)</f>
+      <c r="X9" s="2">
+        <f>_xlfn.XMATCH(V9,$U$9:$U$22,,1)</f>
+        <v>1</v>
+      </c>
+      <c r="Y9" s="2" cm="1">
+        <f t="array" ref="Y9">INDEX(_xlfn.ANCHORARRAY($T$9),W9)</f>
         <v>1004</v>
       </c>
-      <c r="X9" s="2" cm="1">
-        <f t="array" ref="X9">INDEX(_xlfn.ANCHORARRAY($R$9),V9)</f>
+      <c r="Z9" s="2" cm="1">
+        <f t="array" ref="Z9">INDEX(_xlfn.ANCHORARRAY($T$9),X9)</f>
         <v>1001</v>
       </c>
-      <c r="Y9" s="2" t="str">
-        <f>IF(W9&lt;&gt;X9,X9&amp;"-"&amp;W9,TEXT(W9,"0"))</f>
+      <c r="AA9" s="2" t="str">
+        <f>IF(Y9&lt;&gt;Z9,Z9&amp;"-"&amp;Y9,TEXT(Y9,"0"))</f>
         <v>1001-1004</v>
       </c>
     </row>
-    <row r="10" spans="2:25" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:27" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B10" s="9">
         <v>1015</v>
       </c>
       <c r="C10"/>
       <c r="D10"/>
-      <c r="J10"/>
-      <c r="K10" s="28">
+      <c r="J10">
+        <f t="shared" ref="J10:J22" si="1">SUM(K10+J9)</f>
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <f t="shared" ref="K10:K22" si="2">IF(T10-T9&gt;1,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="L10"/>
+      <c r="M10" s="27">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="L10" s="2">
-        <f t="shared" ref="L10:L22" si="1">R11-R10</f>
-        <v>1</v>
-      </c>
-      <c r="M10" s="5">
-        <f t="shared" ref="M10:M22" si="2">N10+M9</f>
-        <v>0</v>
-      </c>
-      <c r="N10" s="5">
-        <f t="shared" ref="N10:N22" si="3">--OR(O10,NOT(OR(O10:Q10)))</f>
-        <v>0</v>
-      </c>
-      <c r="O10" s="5" t="b">
-        <f t="shared" ref="O10:O22" si="4">AND(R11-R10=1,NOT(P10))</f>
-        <v>0</v>
-      </c>
-      <c r="P10" s="2" t="b">
-        <f t="shared" ref="P10:P22" si="5">AND((R11-R10)=1,R10-R9=1)</f>
-        <v>1</v>
-      </c>
-      <c r="Q10" s="2" t="b">
-        <f t="shared" ref="Q10:Q22" si="6">AND((R11-R10&lt;&gt;1),OR(O9,P9))</f>
-        <v>0</v>
-      </c>
-      <c r="R10" s="2">
+      <c r="N10" s="2">
+        <f t="shared" ref="N10:N22" si="3">T11-T10</f>
+        <v>1</v>
+      </c>
+      <c r="O10" s="5">
+        <f t="shared" ref="O10:O22" si="4">P10+O9</f>
+        <v>0</v>
+      </c>
+      <c r="P10" s="5">
+        <f t="shared" ref="P10:P22" si="5">--OR(Q10,NOT(OR(Q10:S10)))</f>
+        <v>0</v>
+      </c>
+      <c r="Q10" s="5" t="b">
+        <f t="shared" ref="Q10:Q22" si="6">AND(T11-T10=1,NOT(R10))</f>
+        <v>0</v>
+      </c>
+      <c r="R10" s="2" t="b">
+        <f t="shared" ref="R10:R22" si="7">AND((T11-T10)=1,T10-T9=1)</f>
+        <v>1</v>
+      </c>
+      <c r="S10" s="2" t="b">
+        <f t="shared" ref="S10:S22" si="8">AND((T11-T10&lt;&gt;1),OR(Q9,R9))</f>
+        <v>0</v>
+      </c>
+      <c r="T10" s="2">
         <v>1002</v>
       </c>
-      <c r="S10" s="5">
-        <f t="shared" ref="S10:S22" si="7">M10</f>
-        <v>0</v>
-      </c>
-      <c r="T10" s="2">
-        <v>1</v>
-      </c>
-      <c r="U10" s="2">
-        <f t="shared" ref="U10:U13" si="8">_xlfn.XMATCH(T10,$S$9:$S$22,,-1)</f>
+      <c r="U10" s="5">
+        <f t="shared" ref="U10:U22" si="9">O10</f>
+        <v>0</v>
+      </c>
+      <c r="V10" s="2">
+        <v>1</v>
+      </c>
+      <c r="W10" s="2">
+        <f t="shared" ref="W10:W13" si="10">_xlfn.XMATCH(V10,$U$9:$U$22,,-1)</f>
         <v>5</v>
       </c>
-      <c r="V10" s="2">
-        <f t="shared" ref="V10:V13" si="9">_xlfn.XMATCH(T10,$S$9:$S$22,,1)</f>
+      <c r="X10" s="2">
+        <f t="shared" ref="X10:X13" si="11">_xlfn.XMATCH(V10,$U$9:$U$22,,1)</f>
         <v>5</v>
       </c>
-      <c r="W10" s="2" cm="1">
-        <f t="array" ref="W10">INDEX(_xlfn.ANCHORARRAY($R$9),U10)</f>
+      <c r="Y10" s="2" cm="1">
+        <f t="array" ref="Y10">INDEX(_xlfn.ANCHORARRAY($T$9),W10)</f>
         <v>1006</v>
       </c>
-      <c r="X10" s="2" cm="1">
-        <f t="array" ref="X10">INDEX(_xlfn.ANCHORARRAY($R$9),V10)</f>
+      <c r="Z10" s="2" cm="1">
+        <f t="array" ref="Z10">INDEX(_xlfn.ANCHORARRAY($T$9),X10)</f>
         <v>1006</v>
       </c>
-      <c r="Y10" s="2" t="str">
-        <f t="shared" ref="Y10:Y13" si="10">IF(W10&lt;&gt;X10,X10&amp;"-"&amp;W10,TEXT(W10,"0"))</f>
+      <c r="AA10" s="2" t="str">
+        <f t="shared" ref="AA10:AA13" si="12">IF(Y10&lt;&gt;Z10,Z10&amp;"-"&amp;Y10,TEXT(Y10,"0"))</f>
         <v>1006</v>
       </c>
     </row>
-    <row r="11" spans="2:25" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:27" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B11" s="12">
         <v>1010</v>
       </c>
       <c r="D11"/>
-      <c r="J11"/>
-      <c r="K11" s="28">
+      <c r="J11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L11"/>
+      <c r="M11" s="27">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="L11" s="2">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="M11" s="5">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N11" s="5">
+      <c r="N11" s="2">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="O11" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="O11" s="5">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="P11" s="2" t="b">
+      <c r="P11" s="5">
         <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="Q11" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="5" t="b">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="R11" s="2">
+      <c r="R11" s="2" t="b">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="S11" s="2" t="b">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="T11" s="2">
         <v>1003</v>
       </c>
-      <c r="S11" s="5">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="T11" s="2">
-        <v>2</v>
-      </c>
-      <c r="U11" s="2">
-        <f t="shared" si="8"/>
+      <c r="U11" s="5">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="V11" s="2">
+        <v>2</v>
+      </c>
+      <c r="W11" s="2">
+        <f t="shared" si="10"/>
         <v>11</v>
       </c>
-      <c r="V11" s="2">
-        <f t="shared" si="9"/>
+      <c r="X11" s="2">
+        <f t="shared" si="11"/>
         <v>6</v>
       </c>
-      <c r="W11" s="2" cm="1">
-        <f t="array" ref="W11">INDEX(_xlfn.ANCHORARRAY($R$9),U11)</f>
+      <c r="Y11" s="2" cm="1">
+        <f t="array" ref="Y11">INDEX(_xlfn.ANCHORARRAY($T$9),W11)</f>
         <v>1013</v>
       </c>
-      <c r="X11" s="2" cm="1">
-        <f t="array" ref="X11">INDEX(_xlfn.ANCHORARRAY($R$9),V11)</f>
+      <c r="Z11" s="2" cm="1">
+        <f t="array" ref="Z11">INDEX(_xlfn.ANCHORARRAY($T$9),X11)</f>
         <v>1008</v>
       </c>
-      <c r="Y11" s="2" t="str">
-        <f t="shared" si="10"/>
+      <c r="AA11" s="2" t="str">
+        <f t="shared" si="12"/>
         <v>1008-1013</v>
       </c>
     </row>
-    <row r="12" spans="2:25" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:27" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B12" s="12">
         <v>1009</v>
       </c>
       <c r="D12"/>
-      <c r="J12"/>
-      <c r="K12" s="28">
+      <c r="J12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L12"/>
+      <c r="M12" s="27">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="L12" s="2">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="M12" s="5">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N12" s="5">
+      <c r="N12" s="2">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="O12" s="5" t="b">
+        <v>2</v>
+      </c>
+      <c r="O12" s="5">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="P12" s="2" t="b">
+      <c r="P12" s="5">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="Q12" s="2" t="b">
+      <c r="Q12" s="5" t="b">
         <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="R12" s="2">
+        <v>0</v>
+      </c>
+      <c r="R12" s="2" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="S12" s="2" t="b">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="T12" s="2">
         <v>1004</v>
       </c>
-      <c r="S12" s="5">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="T12" s="2">
+      <c r="U12" s="5">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="V12" s="2">
         <v>3</v>
       </c>
-      <c r="U12" s="2">
-        <f t="shared" si="8"/>
+      <c r="W12" s="2">
+        <f t="shared" si="10"/>
         <v>13</v>
       </c>
-      <c r="V12" s="2">
-        <f t="shared" si="9"/>
+      <c r="X12" s="2">
+        <f t="shared" si="11"/>
         <v>12</v>
       </c>
-      <c r="W12" s="2" cm="1">
-        <f t="array" ref="W12">INDEX(_xlfn.ANCHORARRAY($R$9),U12)</f>
+      <c r="Y12" s="2" cm="1">
+        <f t="array" ref="Y12">INDEX(_xlfn.ANCHORARRAY($T$9),W12)</f>
         <v>1016</v>
       </c>
-      <c r="X12" s="2" cm="1">
-        <f t="array" ref="X12">INDEX(_xlfn.ANCHORARRAY($R$9),V12)</f>
+      <c r="Z12" s="2" cm="1">
+        <f t="array" ref="Z12">INDEX(_xlfn.ANCHORARRAY($T$9),X12)</f>
         <v>1015</v>
       </c>
-      <c r="Y12" s="2" t="str">
-        <f t="shared" si="10"/>
+      <c r="AA12" s="2" t="str">
+        <f t="shared" si="12"/>
         <v>1015-1016</v>
       </c>
     </row>
-    <row r="13" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B13" s="12">
         <v>1012</v>
       </c>
       <c r="C13" s="2"/>
-      <c r="K13" s="27">
+      <c r="J13">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="M13" s="26">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="L13" s="2">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="M13" s="5">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="N13" s="5">
+      <c r="N13" s="2">
         <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="O13" s="5" t="b">
+        <v>2</v>
+      </c>
+      <c r="O13" s="5">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="P13" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="P13" s="5">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="Q13" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q13" s="5" t="b">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="R13">
+      <c r="R13" s="2" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="S13" s="2" t="b">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="T13">
         <v>1006</v>
       </c>
-      <c r="S13" s="5">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="T13">
+      <c r="U13" s="5">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="V13">
         <v>4</v>
       </c>
-      <c r="U13" s="2">
-        <f t="shared" si="8"/>
+      <c r="W13" s="2">
+        <f t="shared" si="10"/>
         <v>14</v>
       </c>
-      <c r="V13" s="2">
-        <f t="shared" si="9"/>
+      <c r="X13" s="2">
+        <f t="shared" si="11"/>
         <v>14</v>
       </c>
-      <c r="W13" s="2" cm="1">
-        <f t="array" ref="W13">INDEX(_xlfn.ANCHORARRAY($R$9),U13)</f>
+      <c r="Y13" s="2" cm="1">
+        <f t="array" ref="Y13">INDEX(_xlfn.ANCHORARRAY($T$9),W13)</f>
         <v>1018</v>
       </c>
-      <c r="X13" s="2" cm="1">
-        <f t="array" ref="X13">INDEX(_xlfn.ANCHORARRAY($R$9),V13)</f>
+      <c r="Z13" s="2" cm="1">
+        <f t="array" ref="Z13">INDEX(_xlfn.ANCHORARRAY($T$9),X13)</f>
         <v>1018</v>
       </c>
-      <c r="Y13" s="2" t="str">
-        <f t="shared" si="10"/>
+      <c r="AA13" s="2" t="str">
+        <f t="shared" si="12"/>
         <v>1018</v>
       </c>
     </row>
-    <row r="14" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B14" s="11">
         <v>1004</v>
       </c>
       <c r="C14" s="2"/>
-      <c r="K14" s="29">
+      <c r="J14">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="M14" s="28">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="L14" s="2">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="M14" s="5">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="N14" s="5">
+      <c r="N14" s="2">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="O14" s="5" t="b">
+      <c r="O14" s="5">
         <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="P14" s="2" t="b">
+        <v>2</v>
+      </c>
+      <c r="P14" s="5">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="Q14" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q14" s="5" t="b">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="R14">
+        <v>1</v>
+      </c>
+      <c r="R14" s="2" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="S14" s="2" t="b">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="T14">
         <v>1008</v>
       </c>
-      <c r="S14" s="5">
-        <f t="shared" si="7"/>
-        <v>2</v>
-      </c>
-      <c r="U14" s="2"/>
-      <c r="V14" s="2"/>
-      <c r="Y14" s="2"/>
-    </row>
-    <row r="15" spans="2:25" x14ac:dyDescent="0.3">
+      <c r="U14" s="5">
+        <f t="shared" si="9"/>
+        <v>2</v>
+      </c>
+      <c r="W14" s="2"/>
+      <c r="X14" s="2"/>
+      <c r="AA14" s="2"/>
+    </row>
+    <row r="15" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B15" s="11">
         <v>1002</v>
       </c>
       <c r="C15" s="2"/>
-      <c r="K15" s="29">
+      <c r="J15">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M15" s="28">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="L15" s="2">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="M15" s="5">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="N15" s="5">
+      <c r="N15" s="2">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="O15" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="O15" s="5">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="P15" s="2" t="b">
+        <v>2</v>
+      </c>
+      <c r="P15" s="5">
         <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="Q15" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="5" t="b">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="R15">
+      <c r="R15" s="2" t="b">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="S15" s="2" t="b">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="T15">
         <v>1009</v>
       </c>
-      <c r="S15" s="5">
-        <f t="shared" si="7"/>
-        <v>2</v>
-      </c>
-      <c r="U15" s="2"/>
-      <c r="V15" s="2"/>
-      <c r="Y15" s="2"/>
-    </row>
-    <row r="16" spans="2:25" x14ac:dyDescent="0.3">
+      <c r="U15" s="5">
+        <f t="shared" si="9"/>
+        <v>2</v>
+      </c>
+      <c r="W15" s="2"/>
+      <c r="X15" s="2"/>
+      <c r="AA15" s="2"/>
+    </row>
+    <row r="16" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B16" s="14">
         <v>1011</v>
       </c>
       <c r="C16" s="2"/>
-      <c r="K16" s="29">
+      <c r="J16">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M16" s="28">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="L16" s="2">
+      <c r="N16" s="2">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="O16" s="5">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="P16" s="5">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="Q16" s="5" t="b">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="R16" s="2" t="b">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="S16" s="2" t="b">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="T16">
+        <v>1010</v>
+      </c>
+      <c r="U16" s="5">
+        <f t="shared" si="9"/>
+        <v>2</v>
+      </c>
+      <c r="W16" s="2"/>
+      <c r="X16" s="2"/>
+      <c r="AA16" s="2"/>
+    </row>
+    <row r="17" spans="9:27" x14ac:dyDescent="0.3">
+      <c r="J17">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="M16" s="5">
+        <v>2</v>
+      </c>
+      <c r="K17">
         <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="N16" s="5">
+        <v>0</v>
+      </c>
+      <c r="M17" s="28">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="N17" s="2">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="O16" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="O17" s="5">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="P16" s="2" t="b">
+        <v>2</v>
+      </c>
+      <c r="P17" s="5">
         <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="Q16" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="5" t="b">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="R16">
-        <v>1010</v>
-      </c>
-      <c r="S16" s="5">
+      <c r="R17" s="2" t="b">
         <f t="shared" si="7"/>
-        <v>2</v>
-      </c>
-      <c r="U16" s="2"/>
-      <c r="V16" s="2"/>
-      <c r="Y16" s="2"/>
-    </row>
-    <row r="17" spans="7:25" x14ac:dyDescent="0.3">
-      <c r="K17" s="29">
+        <v>1</v>
+      </c>
+      <c r="S17" s="2" t="b">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="T17">
+        <v>1011</v>
+      </c>
+      <c r="U17" s="5">
+        <f t="shared" si="9"/>
+        <v>2</v>
+      </c>
+      <c r="W17" s="2"/>
+      <c r="X17" s="2"/>
+      <c r="AA17" s="2"/>
+    </row>
+    <row r="18" spans="9:27" x14ac:dyDescent="0.3">
+      <c r="J18">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="K18">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M18" s="28">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="L17" s="2">
+      <c r="N18" s="2">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="O18" s="5">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="P18" s="5">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="Q18" s="5" t="b">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="R18" s="2" t="b">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="S18" s="2" t="b">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="T18">
+        <v>1012</v>
+      </c>
+      <c r="U18" s="5">
+        <f t="shared" si="9"/>
+        <v>2</v>
+      </c>
+      <c r="W18" s="2"/>
+      <c r="X18" s="2"/>
+      <c r="AA18" s="2"/>
+    </row>
+    <row r="19" spans="9:27" x14ac:dyDescent="0.3">
+      <c r="J19">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="M17" s="5">
+        <v>2</v>
+      </c>
+      <c r="K19">
         <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="N17" s="5">
+        <v>0</v>
+      </c>
+      <c r="M19" s="28">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="N19" s="2">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="O17" s="5" t="b">
+        <v>2</v>
+      </c>
+      <c r="O19" s="5">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="P17" s="2" t="b">
+        <v>2</v>
+      </c>
+      <c r="P19" s="5">
         <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="Q17" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q19" s="5" t="b">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="R17">
-        <v>1011</v>
-      </c>
-      <c r="S17" s="5">
+      <c r="R19" s="2" t="b">
         <f t="shared" si="7"/>
-        <v>2</v>
-      </c>
-      <c r="U17" s="2"/>
-      <c r="V17" s="2"/>
-      <c r="Y17" s="2"/>
-    </row>
-    <row r="18" spans="7:25" x14ac:dyDescent="0.3">
-      <c r="K18" s="29">
+        <v>0</v>
+      </c>
+      <c r="S19" s="2" t="b">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="T19">
+        <v>1013</v>
+      </c>
+      <c r="U19" s="5">
+        <f t="shared" si="9"/>
+        <v>2</v>
+      </c>
+      <c r="W19" s="2"/>
+      <c r="X19" s="2"/>
+      <c r="AA19" s="2"/>
+    </row>
+    <row r="20" spans="9:27" x14ac:dyDescent="0.3">
+      <c r="J20">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="K20">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="M20" s="29">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="L18" s="2">
+        <v>2</v>
+      </c>
+      <c r="N20" s="2">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="O20" s="5">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="P20" s="5">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="Q20" s="5" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="R20" s="2" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="S20" s="2" t="b">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="T20">
+        <v>1015</v>
+      </c>
+      <c r="U20" s="5">
+        <f t="shared" si="9"/>
+        <v>3</v>
+      </c>
+      <c r="W20" s="2"/>
+      <c r="X20" s="2"/>
+      <c r="AA20" s="2"/>
+    </row>
+    <row r="21" spans="9:27" x14ac:dyDescent="0.3">
+      <c r="J21">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="M18" s="5">
+        <v>3</v>
+      </c>
+      <c r="K21">
         <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="N18" s="5">
+        <v>0</v>
+      </c>
+      <c r="M21" s="29">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="N21" s="2">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="O18" s="5" t="b">
+        <v>2</v>
+      </c>
+      <c r="O21" s="5">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="P18" s="2" t="b">
+        <v>3</v>
+      </c>
+      <c r="P21" s="5">
         <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="Q18" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q21" s="5" t="b">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="R18">
-        <v>1012</v>
-      </c>
-      <c r="S18" s="5">
+      <c r="R21" s="2" t="b">
         <f t="shared" si="7"/>
-        <v>2</v>
-      </c>
-      <c r="U18" s="2"/>
-      <c r="V18" s="2"/>
-      <c r="Y18" s="2"/>
-    </row>
-    <row r="19" spans="7:25" x14ac:dyDescent="0.3">
-      <c r="K19" s="29">
+        <v>0</v>
+      </c>
+      <c r="S21" s="2" t="b">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="T21">
+        <v>1016</v>
+      </c>
+      <c r="U21" s="5">
+        <f t="shared" si="9"/>
+        <v>3</v>
+      </c>
+      <c r="W21" s="2"/>
+      <c r="X21" s="2"/>
+      <c r="AA21" s="2"/>
+    </row>
+    <row r="22" spans="9:27" x14ac:dyDescent="0.3">
+      <c r="J22">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="K22">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="M22" s="30">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="L19" s="2">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="M19" s="5">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="N19" s="5">
+        <v>2</v>
+      </c>
+      <c r="N22" s="2">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="O19" s="5" t="b">
+      <c r="O22" s="5">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="P19" s="2" t="b">
+        <v>4</v>
+      </c>
+      <c r="P22" s="5">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="Q19" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q22" s="5" t="b">
         <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="R19">
-        <v>1013</v>
-      </c>
-      <c r="S19" s="5">
+        <v>0</v>
+      </c>
+      <c r="R22" s="2" t="b">
         <f t="shared" si="7"/>
-        <v>2</v>
-      </c>
-      <c r="U19" s="2"/>
-      <c r="V19" s="2"/>
-      <c r="Y19" s="2"/>
-    </row>
-    <row r="20" spans="7:25" x14ac:dyDescent="0.3">
-      <c r="K20" s="30">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="L20" s="2">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="M20" s="5">
-        <f t="shared" si="2"/>
-        <v>3</v>
-      </c>
-      <c r="N20" s="5">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="O20" s="5" t="b">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="P20" s="2" t="b">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="Q20" s="2" t="b">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="R20">
-        <v>1015</v>
-      </c>
-      <c r="S20" s="5">
-        <f t="shared" si="7"/>
-        <v>3</v>
-      </c>
-      <c r="U20" s="2"/>
-      <c r="V20" s="2"/>
-      <c r="Y20" s="2"/>
-    </row>
-    <row r="21" spans="7:25" x14ac:dyDescent="0.3">
-      <c r="K21" s="30">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="L21" s="2">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="M21" s="5">
-        <f t="shared" si="2"/>
-        <v>3</v>
-      </c>
-      <c r="N21" s="5">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="O21" s="5" t="b">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="P21" s="2" t="b">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="Q21" s="2" t="b">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="R21">
-        <v>1016</v>
-      </c>
-      <c r="S21" s="5">
-        <f t="shared" si="7"/>
-        <v>3</v>
-      </c>
-      <c r="U21" s="2"/>
-      <c r="V21" s="2"/>
-      <c r="Y21" s="2"/>
-    </row>
-    <row r="22" spans="7:25" x14ac:dyDescent="0.3">
-      <c r="K22" s="31">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="L22" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="M22" s="5">
-        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="S22" s="2" t="b">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="T22">
+        <v>1018</v>
+      </c>
+      <c r="U22" s="5">
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
-      <c r="N22" s="5">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="O22" s="5" t="b">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="P22" s="2" t="b">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="Q22" s="2" t="b">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="R22">
+      <c r="W22" s="2"/>
+      <c r="X22" s="2"/>
+      <c r="AA22" s="2"/>
+    </row>
+    <row r="23" spans="9:27" x14ac:dyDescent="0.3">
+      <c r="M23" s="2"/>
+      <c r="P23" s="2"/>
+      <c r="Q23" s="5"/>
+      <c r="R23" s="2"/>
+      <c r="T23" s="6">
         <v>1018</v>
       </c>
-      <c r="S22" s="5">
-        <f t="shared" si="7"/>
-        <v>4</v>
-      </c>
-      <c r="U22" s="2"/>
-      <c r="V22" s="2"/>
-      <c r="Y22" s="2"/>
-    </row>
-    <row r="23" spans="7:25" x14ac:dyDescent="0.3">
-      <c r="G23" cm="1">
-        <f t="array" ref="G23:G39">_xlfn.LET(
-_xlpm.x,_xlfn.VSTACK(0,_xlfn.ANCHORARRAY(R9),100,0),
-_xlpm.x
-)</f>
-        <v>0</v>
-      </c>
-      <c r="K23" s="2"/>
-      <c r="N23" s="2"/>
-      <c r="O23" s="5"/>
-      <c r="P23" s="2"/>
-      <c r="R23" s="6">
-        <v>1018</v>
-      </c>
-      <c r="U23" s="1"/>
-    </row>
-    <row r="24" spans="7:25" x14ac:dyDescent="0.3">
-      <c r="G24">
-        <v>1001</v>
-      </c>
-      <c r="Q24" s="6"/>
-      <c r="T24" s="1"/>
-    </row>
-    <row r="25" spans="7:25" x14ac:dyDescent="0.3">
-      <c r="G25">
-        <v>1002</v>
+      <c r="W23" s="1"/>
+    </row>
+    <row r="24" spans="9:27" x14ac:dyDescent="0.3">
+      <c r="R24" s="6"/>
+      <c r="U24" s="1"/>
+    </row>
+    <row r="25" spans="9:27" x14ac:dyDescent="0.3">
+      <c r="I25" s="10" t="str" cm="1">
+        <f t="array" ref="I25:I30" xml:space="preserve"> _xlfn.LET(
+      _xlpm.x, _xlfn.VSTACK(1000, _nR),
+      _xlpm.y, IF(INDEX(_xlpm.x, _xlfn.SEQUENCE(ROWS(_xlpm.x) - 1, 1, 2)) - INDEX(_xlpm.x, _xlfn.SEQUENCE(ROWS(_xlpm.x) - 1, 1, 1)) &gt; 1, 1, 0),
+      _xlpm.z, _xlfn.SCAN(0, _xlpm.y, _xlfn.LAMBDA(_xlpm.a,_xlpm.v, _xlpm.a + _xlpm.v)),
+      _xlpm.q, _xlfn.UNIQUE(_xlpm.z),
+      _xlpm._x1, _xlfn.XMATCH(_xlpm.q, _xlpm.z, , 1),
+      _xlpm._x0, _xlfn.XMATCH(_xlpm.q, _xlpm.z, , -1),
+      _xlpm._y0, INDEX(_nR, _xlpm._x0),
+      _xlpm._y1, INDEX(_nR, _xlpm._x1),
+      _xlpm._mm, IF(_xlpm._y1 &lt;&gt; _xlpm._y0, _xlpm._y1 &amp; "-" &amp; _xlpm._y0, TEXT(_xlpm._y0, "0")),
+      _xlfn.VSTACK(
+             "Product ID",
+             _xlpm._mm
+      )
+  )</f>
+        <v>Product ID</v>
       </c>
       <c r="P25" s="6"/>
       <c r="S25" s="1"/>
     </row>
-    <row r="26" spans="7:25" x14ac:dyDescent="0.3">
-      <c r="G26">
-        <v>1003</v>
+    <row r="26" spans="9:27" x14ac:dyDescent="0.3">
+      <c r="I26" s="15" t="str">
+        <v>1001-1004</v>
+      </c>
+      <c r="K26" t="b" cm="1">
+        <f t="array" ref="K26:K30">I26:I30=AA9:AA13</f>
+        <v>1</v>
       </c>
       <c r="P26" s="6"/>
       <c r="S26" s="1"/>
     </row>
-    <row r="27" spans="7:25" x14ac:dyDescent="0.3">
-      <c r="G27">
-        <v>1004</v>
+    <row r="27" spans="9:27" x14ac:dyDescent="0.3">
+      <c r="I27" s="16" t="str">
+        <v>1006</v>
+      </c>
+      <c r="K27" t="b">
+        <v>1</v>
       </c>
       <c r="P27" s="6"/>
       <c r="S27" s="1"/>
     </row>
-    <row r="28" spans="7:25" x14ac:dyDescent="0.3">
-      <c r="G28">
-        <v>1006</v>
+    <row r="28" spans="9:27" x14ac:dyDescent="0.3">
+      <c r="I28" s="17" t="str">
+        <v>1008-1013</v>
+      </c>
+      <c r="K28" t="b">
+        <v>1</v>
       </c>
       <c r="P28" s="6"/>
       <c r="S28" s="1"/>
     </row>
-    <row r="29" spans="7:25" x14ac:dyDescent="0.3">
-      <c r="G29">
-        <v>1008</v>
+    <row r="29" spans="9:27" x14ac:dyDescent="0.3">
+      <c r="I29" s="18" t="str">
+        <v>1015-1016</v>
+      </c>
+      <c r="K29" t="b">
+        <v>1</v>
       </c>
       <c r="P29" s="6"/>
       <c r="S29" s="1"/>
     </row>
-    <row r="30" spans="7:25" x14ac:dyDescent="0.3">
-      <c r="G30">
-        <v>1009</v>
+    <row r="30" spans="9:27" x14ac:dyDescent="0.3">
+      <c r="I30" s="19" t="str">
+        <v>1018</v>
+      </c>
+      <c r="K30" t="b">
+        <v>1</v>
       </c>
       <c r="P30" s="6"/>
       <c r="S30" s="1"/>
     </row>
-    <row r="31" spans="7:25" x14ac:dyDescent="0.3">
-      <c r="G31">
-        <v>1010</v>
-      </c>
+    <row r="31" spans="9:27" x14ac:dyDescent="0.3">
       <c r="P31" s="1"/>
       <c r="S31" s="1"/>
     </row>
-    <row r="32" spans="7:25" x14ac:dyDescent="0.3">
-      <c r="G32">
-        <v>1011</v>
-      </c>
+    <row r="32" spans="9:27" x14ac:dyDescent="0.3">
       <c r="P32" s="1"/>
       <c r="S32" s="1"/>
     </row>
-    <row r="33" spans="7:19" x14ac:dyDescent="0.3">
-      <c r="G33">
-        <v>1012</v>
-      </c>
+    <row r="33" spans="16:19" x14ac:dyDescent="0.3">
       <c r="P33" s="1"/>
       <c r="S33" s="1"/>
     </row>
-    <row r="34" spans="7:19" x14ac:dyDescent="0.3">
-      <c r="G34">
-        <v>1013</v>
-      </c>
+    <row r="34" spans="16:19" x14ac:dyDescent="0.3">
       <c r="P34" s="1"/>
       <c r="S34" s="1"/>
     </row>
-    <row r="35" spans="7:19" x14ac:dyDescent="0.3">
-      <c r="G35">
-        <v>1015</v>
-      </c>
+    <row r="35" spans="16:19" x14ac:dyDescent="0.3">
       <c r="P35" s="1"/>
       <c r="S35" s="1"/>
     </row>
-    <row r="36" spans="7:19" x14ac:dyDescent="0.3">
-      <c r="G36">
-        <v>1016</v>
-      </c>
+    <row r="36" spans="16:19" x14ac:dyDescent="0.3">
       <c r="P36" s="1"/>
       <c r="S36" s="1"/>
     </row>
-    <row r="37" spans="7:19" x14ac:dyDescent="0.3">
-      <c r="G37">
-        <v>1018</v>
-      </c>
+    <row r="37" spans="16:19" x14ac:dyDescent="0.3">
       <c r="P37" s="1"/>
       <c r="S37" s="1"/>
     </row>
-    <row r="38" spans="7:19" x14ac:dyDescent="0.3">
-      <c r="G38">
-        <v>100</v>
-      </c>
+    <row r="38" spans="16:19" x14ac:dyDescent="0.3">
       <c r="P38" s="1"/>
       <c r="S38" s="1"/>
     </row>
-    <row r="39" spans="7:19" x14ac:dyDescent="0.3">
-      <c r="G39">
-        <v>0</v>
-      </c>
+    <row r="39" spans="16:19" x14ac:dyDescent="0.3">
       <c r="P39" s="1"/>
       <c r="S39" s="1"/>
     </row>
-    <row r="40" spans="7:19" x14ac:dyDescent="0.3">
+    <row r="40" spans="16:19" x14ac:dyDescent="0.3">
       <c r="P40" s="1"/>
       <c r="S40" s="1"/>
     </row>
-    <row r="41" spans="7:19" x14ac:dyDescent="0.3">
+    <row r="41" spans="16:19" x14ac:dyDescent="0.3">
       <c r="S41" s="1"/>
     </row>
-    <row r="42" spans="7:19" x14ac:dyDescent="0.3">
+    <row r="42" spans="16:19" x14ac:dyDescent="0.3">
       <c r="S42" s="1"/>
     </row>
-    <row r="43" spans="7:19" x14ac:dyDescent="0.3">
+    <row r="43" spans="16:19" x14ac:dyDescent="0.3">
       <c r="S43" s="1"/>
     </row>
-    <row r="44" spans="7:19" x14ac:dyDescent="0.3">
+    <row r="44" spans="16:19" x14ac:dyDescent="0.3">
       <c r="S44" s="1"/>
     </row>
-    <row r="45" spans="7:19" x14ac:dyDescent="0.3">
+    <row r="45" spans="16:19" x14ac:dyDescent="0.3">
       <c r="S45" s="1"/>
     </row>
-    <row r="46" spans="7:19" x14ac:dyDescent="0.3">
+    <row r="46" spans="16:19" x14ac:dyDescent="0.3">
       <c r="S46" s="1"/>
     </row>
-    <row r="47" spans="7:19" x14ac:dyDescent="0.3">
+    <row r="47" spans="16:19" x14ac:dyDescent="0.3">
       <c r="S47" s="1"/>
     </row>
-    <row r="48" spans="7:19" x14ac:dyDescent="0.3">
+    <row r="48" spans="16:19" x14ac:dyDescent="0.3">
       <c r="S48" s="1"/>
     </row>
     <row r="49" spans="19:19" x14ac:dyDescent="0.3">

</xml_diff>